<commit_message>
working on remixing data
</commit_message>
<xml_diff>
--- a/xls/subject_author_analysis.xlsx
+++ b/xls/subject_author_analysis.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfoasberg\Desktop\ProjectTRIKE\American_Literature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfoasberg\Desktop\ProjectTRIKE\Son_of_Am_Lit\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="99">
   <si>
     <t>Apess, William (1798-1839)</t>
   </si>
@@ -345,6 +346,9 @@
   </si>
   <si>
     <t>Polish, Jewish immigrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender </t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1190,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -1548,11 +1552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1569,7 @@
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1585,7 +1589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1602,7 +1606,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1615,8 +1619,11 @@
       <c r="D3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1630,7 +1637,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1644,7 +1651,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1658,7 +1665,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1672,7 +1679,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1686,7 +1693,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1700,7 +1707,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1714,7 +1721,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1731,7 +1738,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1748,7 +1755,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1762,7 +1769,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1776,7 +1783,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1793,7 +1800,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -2916,10 +2923,547 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1950</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1980</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
reorganizing for website structure
</commit_message>
<xml_diff>
--- a/xls/subject_author_analysis.xlsx
+++ b/xls/subject_author_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId7"/>
+    <pivotCache cacheId="5" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -664,7 +664,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -955,11 +954,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="269533728"/>
-        <c:axId val="269534288"/>
+        <c:axId val="262188672"/>
+        <c:axId val="262189232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="269533728"/>
+        <c:axId val="262188672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269534288"/>
+        <c:crossAx val="262189232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,7 +1009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="269534288"/>
+        <c:axId val="262189232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1060,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269533728"/>
+        <c:crossAx val="262188672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1075,7 +1074,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1182,7 +1180,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1473,11 +1470,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="265247792"/>
-        <c:axId val="265241072"/>
+        <c:axId val="257449216"/>
+        <c:axId val="257449776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="265247792"/>
+        <c:axId val="257449216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,7 +1517,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="265241072"/>
+        <c:crossAx val="257449776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1528,7 +1525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="265241072"/>
+        <c:axId val="257449776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,7 +1576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="265247792"/>
+        <c:crossAx val="257449216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1593,7 +1590,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1828,11 +1824,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="266099200"/>
-        <c:axId val="266100320"/>
+        <c:axId val="257452576"/>
+        <c:axId val="257535232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="266099200"/>
+        <c:axId val="257452576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="266100320"/>
+        <c:crossAx val="257535232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1883,7 +1879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="266100320"/>
+        <c:axId val="257535232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,7 +1930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="266099200"/>
+        <c:crossAx val="257452576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2123,11 +2119,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="258318880"/>
-        <c:axId val="258320560"/>
+        <c:axId val="257537472"/>
+        <c:axId val="257538032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="258318880"/>
+        <c:axId val="257537472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2170,7 +2166,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="258320560"/>
+        <c:crossAx val="257538032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2178,7 +2174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="258320560"/>
+        <c:axId val="257538032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,7 +2225,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="258318880"/>
+        <c:crossAx val="257537472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2323,7 +2319,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2518,8 +2513,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="269142080"/>
-        <c:axId val="318970832"/>
+        <c:axId val="257574336"/>
+        <c:axId val="257574896"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2612,7 +2607,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="269142080"/>
+        <c:axId val="257574336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,7 +2650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318970832"/>
+        <c:crossAx val="257574896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2663,7 +2658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="318970832"/>
+        <c:axId val="257574896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2714,7 +2709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269142080"/>
+        <c:crossAx val="257574336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2728,7 +2723,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6420,7 +6414,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -6784,9 +6778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D89" sqref="A1:D89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11173,8 +11167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>